<commit_message>
added variables to data spreadsheet intro page
</commit_message>
<xml_diff>
--- a/example-weights-spreadsheets/data/simulation-1-weights-consolidated.xlsx
+++ b/example-weights-spreadsheets/data/simulation-1-weights-consolidated.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,9 +436,121 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
-          <t>The following sheets show the magnitude of each weight over time. The rows represent each weight, and the columns are epochs. Note that some seeds may have fewer epochs than others.</t>
+          <t>simulationTypeNumber</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>seed</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>learning_rate</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>n_pattern</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>n_pattern_features</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>max_epochs</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>energy_exponent</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>preset_simulation</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>weights_initialised_as</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>cache_algorithm</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>max_size_of_transient_memory</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>maintenance_cost_of_transient_memory</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Decay rate of transient memory</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F2" t="n">
+        <v>200</v>
+      </c>
+      <c r="G2" t="n">
+        <v>200</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>zeros</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>local-global</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>1</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>The following sheets show each weight over time. The rows represent each weight, and the columns are epochs. Note that some seeds may have fewer epochs than others.</t>
         </is>
       </c>
     </row>

</xml_diff>